<commit_message>
Space in '_Prev', revision 3 digit bug
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/nishantnaresh_meher_dxc_com/Documents/Documents/git_workspace/c_plus_plus_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="301" documentId="8_{BF3E1325-0CC9-47E8-BCC0-4DA2D55A3C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3D3238B-F15B-4561-8691-980A703B7079}"/>
+  <xr:revisionPtr revIDLastSave="309" documentId="8_{BF3E1325-0CC9-47E8-BCC0-4DA2D55A3C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96F945C9-43FC-4A4E-B502-BC1187C5D139}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-1920" windowWidth="30936" windowHeight="16896" xr2:uid="{AEFA6787-76B0-4AFD-9082-33A24F81C1B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>File Name</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Test-1 [ 8/30 ]</t>
+  </si>
+  <si>
+    <t>Test-3 山田さんと</t>
+  </si>
+  <si>
+    <t>_Prev空間(1っ回目だけ）</t>
   </si>
 </sst>
 </file>
@@ -667,7 +673,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -772,7 +778,14 @@
     </row>
     <row r="5" spans="1:10">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="H5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -862,7 +875,7 @@
       <c r="B19" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="4"/>
@@ -879,6 +892,7 @@
       <c r="B20" t="s">
         <v>17</v>
       </c>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:10">
       <c r="B21" t="s">

</xml_diff>

<commit_message>
Final just make sure the identifier has new 3 digits
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/nishantnaresh_meher_dxc_com/Documents/Documents/git_workspace/c_plus_plus_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="309" documentId="8_{BF3E1325-0CC9-47E8-BCC0-4DA2D55A3C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96F945C9-43FC-4A4E-B502-BC1187C5D139}"/>
+  <xr:revisionPtr revIDLastSave="325" documentId="8_{BF3E1325-0CC9-47E8-BCC0-4DA2D55A3C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50CF8CA4-67C1-435F-B464-B459AF9C4598}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-1920" windowWidth="30936" windowHeight="16896" xr2:uid="{AEFA6787-76B0-4AFD-9082-33A24F81C1B1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AEFA6787-76B0-4AFD-9082-33A24F81C1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
   <si>
     <t>File Name</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>_Prev空間(1っ回目だけ）</t>
+  </si>
+  <si>
+    <t>Test-4 [ 8/31 ]</t>
+  </si>
+  <si>
+    <t>const Vi_Version DasMLoadData_Version        ("DasMLoadData",   "2021/12/05", "000", "01", "RELS_DASMLOADDATA_000-01", "", "hp");</t>
   </si>
 </sst>
 </file>
@@ -253,7 +259,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
@@ -262,6 +268,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -281,96 +290,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2263140</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle: Single Corner Rounded 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57F59751-09AA-2BE5-A72E-110D1ECD07BC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="160020" y="632460"/>
-          <a:ext cx="2103120" cy="1179195"/>
-        </a:xfrm>
-        <a:prstGeom prst="round1Rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>_Prev</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" baseline="0"/>
-            <a:t>の行列に </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>"//</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> const Vi_Version"</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-          </a:br>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" baseline="0"/>
-            <a:t>メインバージョンアップデートの時空間を入ること。</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -673,7 +592,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -682,7 +601,7 @@
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="52.42578125" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" customWidth="1"/>
     <col min="6" max="6" width="29.7109375" customWidth="1"/>
     <col min="7" max="7" width="31.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
@@ -722,7 +641,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="2" spans="1:10" ht="105.75" thickTop="1">
+      <c r="C2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>1</v>
@@ -790,8 +719,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="B6" t="s">
-        <v>19</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10">
       <c r="B7" t="s">
@@ -1037,6 +971,5 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>